<commit_message>
retry with output excel data
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -474,9 +474,233 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Kiwi Kitchens Raw Freeze Dried Cat Treats Salmon Recipe 30g | Catch.com.au</v>
+      </c>
+      <c r="B6" t="str">
+        <v>$6.90</v>
+      </c>
+      <c r="C6" t="str">
+        <v>https://www.catch.com.au/product/kiwi-kitchens-raw-freeze-dried-cat-treats-salmon-recipe-30g-25308308/?sid=Kiwi%20Kitchens%20Raw%20Freeze%20Dried%20Cat%20Treats%20Tuna%20Recipe%2030g&amp;st=32&amp;srtrev=sj-j5nztvbthwy0bjea4vf5q8.click&amp;pid=25308308&amp;sp=2&amp;oid=90790459</v>
+      </c>
+      <c r="D6">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>OsteVit-D One-A-Day Vitamin D3 250 Tabs | Catch.com.au</v>
+      </c>
+      <c r="B7" t="str">
+        <v>$12.99</v>
+      </c>
+      <c r="C7" t="str">
+        <v>https://www.catch.com.au/product/ostevit-d-one-a-day-vitamin-d3-250-tabs-26174042/?sid=Grocery%20%26%20Liquor%20%3E%20Health%20%26%20Wellbeing%20%3E%20Vitamins&amp;st=15&amp;srtrev=sj-32jmfaklbejowe1epxavf2.click&amp;pid=26174042&amp;sp=26&amp;oid=97836753</v>
+      </c>
+      <c r="D7">
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>BeePower Manuka Honey 500+ MGO Lozenges Lemon 40pk | Catch.com.au</v>
+      </c>
+      <c r="B8" t="str">
+        <v>$16.19</v>
+      </c>
+      <c r="C8" t="str">
+        <v>https://www.catch.com.au/product/beepower-manuka-honey-500-mgo-lozenges-lemon-40pk-6119470/?sid=Bee%20Power%20Manuka%20Honey%20Lemon%20Lozenges%20190%20g&amp;st=32&amp;srtrev=sj-dz00y66djmu4900pcp04ht.click&amp;pid=6119470&amp;sp=1&amp;oid=30391320</v>
+      </c>
+      <c r="D8">
+        <v>14.39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Nature's Way Restore Probiotic Daily Health 28 Caps | Catch.com.au</v>
+      </c>
+      <c r="B9" t="str">
+        <v>$16.99</v>
+      </c>
+      <c r="C9" t="str">
+        <v>https://www.catch.com.au/product/natures-way-restore-probiotic-daily-health-28-caps-7728490/?sid=Grocery%20%26%20Liquor%20%3E%20Health%20%26%20Wellbeing%20%3E%20Vitamins&amp;st=15&amp;srtrev=sj-6ak5i7pvzaylbfqzjqwaud.click&amp;pid=7728490&amp;sp=15&amp;oid=39164780</v>
+      </c>
+      <c r="D9">
+        <v>16.99</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Morlife Organic Barley Grass Powder 700g / 350 Serves | Catch.com.au</v>
+      </c>
+      <c r="B10" t="str">
+        <v>$44.95</v>
+      </c>
+      <c r="C10" t="str">
+        <v>https://www.catch.com.au/product/morlife-organic-barley-grass-powder-700g-350-serves-417089/?sid=Grocery%20%26%20Liquor%20%3E%20Health%20%26%20Wellbeing%20%3E%20Diet%20%26%20Slimming&amp;st=15&amp;srtrev=sj-czn49tg62b20v2utysy9ki.click&amp;pid=417089&amp;sp=4&amp;oid=462533</v>
+      </c>
+      <c r="D10">
+        <v>44.95</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>10 x Amazonia RAW Protein Bars Triple Choc Brownie 40g | Catch.com.au</v>
+      </c>
+      <c r="B11" t="str">
+        <v>$35</v>
+      </c>
+      <c r="C11" t="str">
+        <v>https://www.catch.com.au/product/10-x-amazonia-raw-protein-bars-triple-choc-brownie-40g-7730920/?sid=Grocery%20%26%20Liquor%20%3E%20Health%20%26%20Wellbeing%20%3E%20Diet%20%26%20Slimming&amp;st=15&amp;srtrev=sj-d789l8mhvrmo6j3ogjafly.click&amp;pid=7730920&amp;sp=14&amp;oid=39174231</v>
+      </c>
+      <c r="D11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Piksters Interdental Brushes 40pk - Size 1 | Catch.com.au</v>
+      </c>
+      <c r="B12" t="str">
+        <v>$15.53</v>
+      </c>
+      <c r="C12" t="str">
+        <v>https://www.catch.com.au/product/piksters-interdental-brushes-40pk-size-1-6451946/?sid=Beauty%20%3E%20Dental%20%26%20Oral%20Care%20%3E%20Dental%20Floss%20%26%20Picks&amp;st=15&amp;srtrev=sj-c20sj0wcx4c5wub79fwjeg.click&amp;pid=6451946&amp;sp=7&amp;oid=32153160</v>
+      </c>
+      <c r="D12">
+        <v>15.53</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Joseph Joseph 4-Piece Nested Glass Storage Container Set | Catch.com.au</v>
+      </c>
+      <c r="B13" t="str">
+        <v/>
+      </c>
+      <c r="C13" t="str">
+        <v>https://www.catch.com.au/product/joseph-joseph-4-piece-nested-glass-storage-container-set-1911952/?sid=Home%20%26%20Kitchen%20%3E%20Kitchen%20%3E%20Food%20Storage&amp;st=15&amp;srtrev=sj-pqadxjaq4zlnovpbblxvyi.click&amp;pid=1911952&amp;sp=16&amp;oid=11989745</v>
+      </c>
+      <c r="D13">
+        <v>39.2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Avanti 38x27.5cm Potato Bag | Catch.com.au</v>
+      </c>
+      <c r="B14" t="str">
+        <v>$18.95</v>
+      </c>
+      <c r="C14" t="str">
+        <v>https://www.catch.com.au/product/avanti-38x27-5cm-potato-bag-2311534/?sid=Home%20%26%20Kitchen%20%3E%20Kitchen%20%3E%20Food%20Storage&amp;st=15&amp;srtrev=sj-6yezpvrjxrceocdiwerew8.click&amp;pid=2311534&amp;sp=26&amp;oid=75509167</v>
+      </c>
+      <c r="D14">
+        <v>6.69</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Bakemaster 25cm Square Proving Basket | Catch.com.au</v>
+      </c>
+      <c r="B15" t="str">
+        <v>$12.95</v>
+      </c>
+      <c r="C15" t="str">
+        <v>https://www.catch.com.au/product/bakemaster-25cm-square-proving-basket-15086436/?sid=Home%20%26%20Kitchen%20%3E%20Kitchen%20%3E%20Food%20Storage&amp;st=15&amp;srtrev=sj-rud6qpy8iwtc87rrfp4aus.click&amp;pid=15086436&amp;sp=95&amp;oid=75509271</v>
+      </c>
+      <c r="D15">
+        <v>12.95</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Maxwell &amp; Williams 6-Cup BakerMaker Non-Stick Large Muffin Pan | Catch.com.au</v>
+      </c>
+      <c r="B16" t="str">
+        <v>$10.73</v>
+      </c>
+      <c r="C16" t="str">
+        <v>https://www.catch.com.au/product/maxwell-williams-6-cup-bakermaker-non-stick-large-muffin-pan-24879640/?sid=Home%20%26%20Kitchen%20%3E%20Kitchen%20%3E%20Baking&amp;st=15&amp;srtrev=sj-btsljf1lfkv2ocf0yq3d4b.click&amp;pid=24879640&amp;sp=26&amp;oid=87338530</v>
+      </c>
+      <c r="D16">
+        <v>10.73</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Salt &amp; Pepper 12-Piece Napier Dinner Set - Blue | Catch.com.au</v>
+      </c>
+      <c r="B17" t="str">
+        <v>$159.95</v>
+      </c>
+      <c r="C17" t="str">
+        <v>https://www.catch.com.au/product/salt-pepper-12-piece-napier-dinner-set-blue-11801874/?sid=Home%20%26%20Kitchen%20%3E%20Dining%20%3E%20Dinnerware%20%26%20Serveware&amp;st=15&amp;srtrev=sj-8dh3vrcme4ydu8egzc1rr0.click&amp;pid=11801874&amp;sp=1&amp;oid=50160723</v>
+      </c>
+      <c r="D17">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>KitchenAid Soft Touch Can Opener | Catch.com.au</v>
+      </c>
+      <c r="B18" t="str">
+        <v>$14.95</v>
+      </c>
+      <c r="C18" t="str">
+        <v>https://www.catch.com.au/product/kitchenaid-soft-touch-can-opener-5027792/?sid=Home%20%26%20Kitchen%20%3E%20Kitchen&amp;st=15&amp;srtrev=sj-h1anpw2bj8z4ficsigz3kl.click&amp;pid=5027792&amp;sp=23&amp;oid=30079340</v>
+      </c>
+      <c r="D18">
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Maxwell &amp; Williams 5-Piece Cocktail &amp; Co. Lexington Hammered Bar Tool Set | Catch.com.au</v>
+      </c>
+      <c r="B19" t="str">
+        <v>$39</v>
+      </c>
+      <c r="C19" t="str">
+        <v>https://www.catch.com.au/product/maxwell-williams-5-piece-cocktail-co-lexington-hammered-bar-tool-set-24879477/?sid=Home%20%26%20Kitchen%20%3E%20Kitchen&amp;st=15&amp;srtrev=sj-lhzqnuy6g22auci1hachod.click&amp;pid=24879477&amp;sp=34&amp;oid=87337786</v>
+      </c>
+      <c r="D19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>BarCraft Twist Action Wine Bottle Foil Cutter | Catch.com.au</v>
+      </c>
+      <c r="B20" t="str">
+        <v>$4</v>
+      </c>
+      <c r="C20" t="str">
+        <v>https://www.catch.com.au/product/barcraft-twist-action-wine-bottle-foil-cutter-6045358/?sid=Home%20%26%20Kitchen%20%3E%20Kitchen&amp;st=15&amp;srtrev=sj-7dpx2ioq6qwdfqbvlusqjn.click&amp;pid=6045358&amp;sp=44&amp;oid=31733262</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Joseph Joseph Push &amp; Tear Kitchen Roll/Paper Towel Stand | Catch.com.au</v>
+      </c>
+      <c r="B21" t="str">
+        <v>$49.95</v>
+      </c>
+      <c r="C21" t="str">
+        <v>https://www.catch.com.au/product/joseph-joseph-push-tear-kitchen-roll-paper-towel-stand-3904093/?sid=Home%20%26%20Kitchen%20%3E%20Kitchen&amp;st=15&amp;srtrev=sj-pnw3v1vp6p6w2t7xcitwjv.click&amp;pid=3904093&amp;sp=61&amp;oid=29945864</v>
+      </c>
+      <c r="D21">
+        <v>34.95</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>